<commit_message>
Expense-approval model and functionality
</commit_message>
<xml_diff>
--- a/design/User roles and permissions.xlsx
+++ b/design/User roles and permissions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Default user (e.g. stakeholder)</t>
   </si>
@@ -98,59 +98,56 @@
     <t>Can view approved expenses</t>
   </si>
   <si>
+    <t>Can view expenses</t>
+  </si>
+  <si>
+    <t>Journal Entries, approved</t>
+  </si>
+  <si>
+    <t>Can view journal entries</t>
+  </si>
+  <si>
+    <t>Superusers can do everything all other users can do. Additional permissions are listed below.</t>
+  </si>
+  <si>
+    <t>Funds, categories, ledger accounts</t>
+  </si>
+  <si>
+    <t>Expenses, in draft</t>
+  </si>
+  <si>
+    <t>Expenses, submitted for approval</t>
+  </si>
+  <si>
+    <t>Journal Entries, in draft</t>
+  </si>
+  <si>
+    <t>Journal Entries, submitted for approval</t>
+  </si>
+  <si>
+    <t>Can view, create, edit and delete journal entries
+Can submit journal entries for approval</t>
+  </si>
+  <si>
+    <t>Can view, create, edit and delete expenses
+Can submit expenses for approval</t>
+  </si>
+  <si>
     <t>Can view expenses
-If owner, can unsubmit expenses</t>
-  </si>
-  <si>
-    <t>Can view expenses</t>
-  </si>
-  <si>
-    <t>Journal Entries, approved</t>
-  </si>
-  <si>
-    <t>Can delete expenses owned by inactive users</t>
-  </si>
-  <si>
-    <t>Can view journal entries</t>
-  </si>
-  <si>
-    <t>Can view and create expenses
-If owner, can edit and delete expenses
-If owner, can submit expenses for approval</t>
-  </si>
-  <si>
-    <t>Can view and create journal entries
-If owner, can edit and delete journal entries
-If owner, can submit journal entries for approval</t>
+Can unsubmit expenses</t>
   </si>
   <si>
     <t>Can view expenses
-Can approve expenses</t>
+Can approve expenses submitted by someone else</t>
   </si>
   <si>
     <t>Can view journal entries
-Can approve journal entries</t>
-  </si>
-  <si>
-    <t>Can delete journal entries owned by inactive users</t>
-  </si>
-  <si>
-    <t>Superusers can do everything all other users can do. Additional permissions are listed below.</t>
-  </si>
-  <si>
-    <t>Funds, categories, ledger accounts</t>
-  </si>
-  <si>
-    <t>Expenses, in draft</t>
-  </si>
-  <si>
-    <t>Expenses, submitted for approval</t>
-  </si>
-  <si>
-    <t>Journal Entries, in draft</t>
-  </si>
-  <si>
-    <t>Journal Entries, submitted for approval</t>
+Can unsubmit journal entries</t>
+  </si>
+  <si>
+    <t>Can view journal entries
+Can unsubmit journal entries
+Can approve journal entries submitted by someone else</t>
   </si>
 </sst>
 </file>
@@ -509,10 +506,10 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +540,7 @@
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -647,38 +644,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -695,52 +686,46 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -759,7 +744,7 @@
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update user permissions matrix
</commit_message>
<xml_diff>
--- a/design/User roles and permissions.xlsx
+++ b/design/User roles and permissions.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
-  <si>
-    <t>Default user (e.g. stakeholder)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
   <si>
     <t>Bookkeeper</t>
   </si>
@@ -35,27 +32,15 @@
     <t>Accountant</t>
   </si>
   <si>
-    <t>Superuser (i.e. admin)</t>
-  </si>
-  <si>
-    <t>Users</t>
-  </si>
-  <si>
     <t>No access</t>
   </si>
   <si>
     <t>School</t>
   </si>
   <si>
-    <t>Can edit school info</t>
-  </si>
-  <si>
     <t>Students</t>
   </si>
   <si>
-    <t>Terms</t>
-  </si>
-  <si>
     <t>Budgets</t>
   </si>
   <si>
@@ -65,15 +50,6 @@
     <t>Reports</t>
   </si>
   <si>
-    <t>Can view, create, edit, and delete terms</t>
-  </si>
-  <si>
-    <t>Can view and edit budgets</t>
-  </si>
-  <si>
-    <t>Can view, create, edit, and delete users; via admin portal</t>
-  </si>
-  <si>
     <t>Can view reports</t>
   </si>
   <si>
@@ -83,9 +59,6 @@
     <t>Can view, create, edit, and delete students</t>
   </si>
   <si>
-    <t>Can view, create, edit, and delete payees</t>
-  </si>
-  <si>
     <t>Can view, create, edit, and delete revenues</t>
   </si>
   <si>
@@ -105,12 +78,6 @@
   </si>
   <si>
     <t>Can view journal entries</t>
-  </si>
-  <si>
-    <t>Superusers can do everything all other users can do. Additional permissions are listed below.</t>
-  </si>
-  <si>
-    <t>Funds, categories, ledger accounts</t>
   </si>
   <si>
     <t>Expenses, in draft</t>
@@ -148,6 +115,45 @@
     <t>Can view journal entries
 Can unsubmit journal entries
 Can approve journal entries submitted by someone else</t>
+  </si>
+  <si>
+    <t>School Superuser</t>
+  </si>
+  <si>
+    <t>Site Superuser (i.e. admin)</t>
+  </si>
+  <si>
+    <t>Default user without other special credentials (e.g. stakeholder)</t>
+  </si>
+  <si>
+    <t>Student Graduating Classes</t>
+  </si>
+  <si>
+    <t>Full access</t>
+  </si>
+  <si>
+    <t>Can create users
+Can grant and revoke school membership to existing users
+Can grant and revoke permissions to school members</t>
+  </si>
+  <si>
+    <t>Can view revenues</t>
+  </si>
+  <si>
+    <t>Can create and delete schools</t>
+  </si>
+  <si>
+    <t>Can view, create, edit, and delete payees
+Can start and terminate contracts</t>
+  </si>
+  <si>
+    <t>Users and Permissions</t>
+  </si>
+  <si>
+    <t>Funds, categories, ledger accounts, departments</t>
+  </si>
+  <si>
+    <t>Can edit school profile settings</t>
   </si>
 </sst>
 </file>
@@ -192,7 +198,60 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -228,13 +287,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E17" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <tableColumns count="5">
-    <tableColumn id="6" name="Module" dataDxfId="4"/>
-    <tableColumn id="2" name="Default user (e.g. stakeholder)" dataDxfId="3"/>
-    <tableColumn id="3" name="Bookkeeper" dataDxfId="2"/>
-    <tableColumn id="4" name="Accountant" dataDxfId="1"/>
-    <tableColumn id="5" name="Superuser (i.e. admin)" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <tableColumns count="6">
+    <tableColumn id="6" name="Module" dataDxfId="10"/>
+    <tableColumn id="2" name="Default user without other special credentials (e.g. stakeholder)" dataDxfId="9"/>
+    <tableColumn id="3" name="Bookkeeper" dataDxfId="8"/>
+    <tableColumn id="4" name="Accountant" dataDxfId="7"/>
+    <tableColumn id="1" name="School Superuser" dataDxfId="5"/>
+    <tableColumn id="5" name="Site Superuser (i.e. admin)" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -503,13 +563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,248 +578,337 @@
     <col min="2" max="2" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="23.28515625" style="1"/>
+    <col min="5" max="5" width="21.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="23.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" ht="30" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="A1:F16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"No access"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="1">

</xml_diff>